<commit_message>
day 10 part 2
</commit_message>
<xml_diff>
--- a/MyDsaSheet.xlsx
+++ b/MyDsaSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="105">
   <si>
     <t>My Dsa Sheet</t>
   </si>
@@ -308,6 +308,30 @@
   </si>
   <si>
     <t>SEE it after completing searching and sorting</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from sorted array</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/remove-duplicate-elements-from-sorted-array/1</t>
+  </si>
+  <si>
+    <t>Keep track of where next unique elements to be placed</t>
+  </si>
+  <si>
+    <t>Check if array is sorted in non decresing order</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/check-if-an-array-is-sorted0701/1</t>
+  </si>
+  <si>
+    <t>Move Zeroes to end</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/move-all-zeroes-to-end-of-array0751/1</t>
+  </si>
+  <si>
+    <t>Initialise the count to keep track of where next non zero elements is to be placed</t>
   </si>
 </sst>
 </file>
@@ -2458,13 +2482,27 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="21">
       <c r="A38" s="11"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="B38" s="12">
+        <v>45117</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="I38" s="13"/>
       <c r="J38" s="15"/>
       <c r="K38" s="5"/>
@@ -2488,12 +2526,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="21">
       <c r="A39" s="11"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
+      <c r="B39" s="12">
+        <v>45117</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
       <c r="J39" s="15"/>
@@ -2518,13 +2568,27 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="21">
       <c r="A40" s="11"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="B40" s="12">
+        <v>45117</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>104</v>
+      </c>
       <c r="I40" s="13"/>
       <c r="J40" s="15"/>
       <c r="K40" s="5"/>

</xml_diff>